<commit_message>
Nu med maedarbejder tabel
</commit_message>
<xml_diff>
--- a/Case/day/Time_Registration_Daily_20220324.xlsx
+++ b/Case/day/Time_Registration_Daily_20220324.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://accobat-my.sharepoint.com/personal/tml_accobat_com/Documents/Skrivebord/Case/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andreasme\Documents\Power_bi\Case\day\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_D0161456C98BB26DB146E47CCE039485BDA6E65D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8ED16B3D-2EC6-49F0-AD4B-CB72CFE76328}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94ACDA2-47E5-4EE5-8109-4E55D20F7241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="4920" windowWidth="17508" windowHeight="17448" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Object19" sheetId="1" r:id="rId1"/>
@@ -188,7 +188,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -206,17 +206,12 @@
       <name val="Aller"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="none"/>
@@ -263,23 +258,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="39" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="39" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="39" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -298,7 +293,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -597,21 +592,21 @@
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="45.69921875"/>
-    <col min="2" max="2" width="9.19921875"/>
+    <col min="1" max="1" width="45.6875"/>
+    <col min="2" max="2" width="9.1875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:2">
+      <c r="B1" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -619,419 +614,419 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:2" ht="15" customHeight="1">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" customHeight="1">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B4" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" customHeight="1">
+      <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="B5" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" customHeight="1">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="B6" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" customHeight="1">
+      <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" customHeight="1">
+      <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" customHeight="1">
+      <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" customHeight="1">
+      <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="B10" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" customHeight="1">
+      <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="B11" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" customHeight="1">
+      <c r="A12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="B12" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" customHeight="1">
+      <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="B13" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15" customHeight="1">
+      <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="B14" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15" customHeight="1">
+      <c r="A15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="B15" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15" customHeight="1">
+      <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="B16" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" customHeight="1">
+      <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="B17" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" customHeight="1">
+      <c r="A18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="B18" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15" customHeight="1">
+      <c r="A19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="B19" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15" customHeight="1">
+      <c r="A20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="B20" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15" customHeight="1">
+      <c r="A21" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="B21" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15" customHeight="1">
+      <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="B22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15" customHeight="1">
+      <c r="A23" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="B23" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15" customHeight="1">
+      <c r="A24" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="B24" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15" customHeight="1">
+      <c r="A25" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="B25" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15" customHeight="1">
+      <c r="A26" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="B26" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15" customHeight="1">
+      <c r="A27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="B27" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15" customHeight="1">
+      <c r="A28" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="B28" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15" customHeight="1">
+      <c r="A29" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="B29" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15" customHeight="1">
+      <c r="A30" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="B30" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15" customHeight="1">
+      <c r="A31" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="B31" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15" customHeight="1">
+      <c r="A32" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="B32" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15" customHeight="1">
+      <c r="A33" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="B33" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15" customHeight="1">
+      <c r="A34" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="B34" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15" customHeight="1">
+      <c r="A35" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="B35" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15" customHeight="1">
+      <c r="A36" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="B36" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15" customHeight="1">
+      <c r="A37" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="B37" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15" customHeight="1">
+      <c r="A38" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="B38" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15" customHeight="1">
+      <c r="A39" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="B39" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15" customHeight="1">
+      <c r="A40" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="B40" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15" customHeight="1">
+      <c r="A41" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="B41" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15" customHeight="1">
+      <c r="A42" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="B42" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15" customHeight="1">
+      <c r="A43" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="B43" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15" customHeight="1">
+      <c r="A44" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="B44" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15" customHeight="1">
+      <c r="A45" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="B45" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15" customHeight="1">
+      <c r="A46" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="B46" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15" customHeight="1">
+      <c r="A47" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="B47" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15" customHeight="1">
+      <c r="A48" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="B48" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15" customHeight="1">
+      <c r="A49" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="B49" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15" customHeight="1">
+      <c r="A50" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B50" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="B50" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15" customHeight="1">
+      <c r="A51" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="B51" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15" customHeight="1">
+      <c r="A52" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B52" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="B52" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15" customHeight="1">
+      <c r="A53" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+      <c r="B53" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15" customHeight="1">
+      <c r="A54" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B54" s="4">
+      <c r="B54" s="3">
         <v>-1</v>
       </c>
     </row>

</xml_diff>